<commit_message>
new features and reworks for totaldb and collaboratedDB
</commit_message>
<xml_diff>
--- a/src/assets/cbd_template.xlsx
+++ b/src/assets/cbd_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wenta\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9615A1A-C979-4DF0-AECA-A3B016340EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B686A955-B877-405D-B00A-BBA04602ABAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22005" yWindow="5655" windowWidth="15045" windowHeight="13890" xr2:uid="{2EDA58DC-2394-48E0-8795-6BFFE67F9773}"/>
+    <workbookView xWindow="7590" yWindow="4350" windowWidth="28800" windowHeight="15345" xr2:uid="{2EDA58DC-2394-48E0-8795-6BFFE67F9773}"/>
   </bookViews>
   <sheets>
     <sheet name="CD_excel" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Handle Name</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Project  Name</t>
+  </si>
+  <si>
+    <t>Linked</t>
   </si>
 </sst>
 </file>
@@ -916,15 +919,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543A6310-A6A5-4E04-8F74-6C59F31FE0F2}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,6 +963,9 @@
       </c>
       <c r="L1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>